<commit_message>
added new dump of KW24D
</commit_message>
<xml_diff>
--- a/dumps/table.xlsx
+++ b/dumps/table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t xml:space="preserve">Platform_name</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">10500000e062eef000000000000000000000000097969902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ffff1000DBD01E69CBD0E196</t>
   </si>
 </sst>
 </file>
@@ -277,18 +280,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="1" sqref="A1:D12 D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.7732793522267"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -425,6 +428,17 @@
         <v>242</v>
       </c>
       <c r="D11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>